<commit_message>
Additional tests & bug fixing
</commit_message>
<xml_diff>
--- a/test/Function/CppUGenMock UTs.xlsx
+++ b/test/Function/CppUGenMock UTs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="130">
   <si>
     <t>VoidReturnNoParameters</t>
   </si>
@@ -361,6 +361,60 @@
   </si>
   <si>
     <t>StringTypedefConstReturnNoParameters</t>
+  </si>
+  <si>
+    <t>VoidReturnStringConstTypedefTypedefParameter</t>
+  </si>
+  <si>
+    <t>VoidReturnStringTypedefConstTypedefParameter</t>
+  </si>
+  <si>
+    <t>VoidReturnStringTypedefTypedefParameter</t>
+  </si>
+  <si>
+    <t>StringTypedefConstTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>StringConstTypedefTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>StringTypedefTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>VoidReturnPrimitiveTypeTypedefConstPointerParameter</t>
+  </si>
+  <si>
+    <t>VoidReturnPrimitiveTypeTypedefPointerParameter</t>
+  </si>
+  <si>
+    <t>VoidReturnConstPrimitiveTypeTypedefPointerParameter</t>
+  </si>
+  <si>
+    <t>PrimitiveTypeTypedefConstPointerReturnNoParameters</t>
+  </si>
+  <si>
+    <t>PrimitiveTypeTypedefPointerReturnNoParameters</t>
+  </si>
+  <si>
+    <t>ConstPrimitiveTypeTypedefPointerReturnNoParameters</t>
+  </si>
+  <si>
+    <t>PrimitiveTypePointerTypedefConstTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>PrimitiveTypePointerTypedefTypedefConstReturnNoParameters</t>
+  </si>
+  <si>
+    <t>PrimitiveTypePointerTypedefTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>ConstPrimitiveTypePointerTypedefTypedefConstReturnNoParameters</t>
+  </si>
+  <si>
+    <t>ConstPrimitiveTypePointerTypedefConstTypedefReturnNoParameters</t>
+  </si>
+  <si>
+    <t>ConstPrimitiveTypePointerTypedefTypedefReturnNoParameters</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M139"/>
+  <dimension ref="B2:M145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="J127" sqref="J127:K127"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="L127" sqref="L127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,7 +2188,9 @@
       <c r="K36" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="L36" s="13"/>
+      <c r="L36" s="13" t="s">
+        <v>122</v>
+      </c>
       <c r="M36" s="13" t="s">
         <v>107</v>
       </c>
@@ -2164,8 +2220,12 @@
       <c r="K37" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L37" s="13"/>
-      <c r="M37" s="13"/>
+      <c r="L37" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="13" t="s">
@@ -2192,8 +2252,12 @@
       <c r="K38" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L38" s="13"/>
-      <c r="M38" s="13"/>
+      <c r="L38" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M38" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="34" t="s">
@@ -2220,8 +2284,12 @@
       <c r="K39" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
+      <c r="L39" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="13" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="13" t="s">
@@ -2248,8 +2316,12 @@
       <c r="K40" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L40" s="13"/>
-      <c r="M40" s="13"/>
+      <c r="L40" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M40" s="13" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="13" t="s">
@@ -2276,8 +2348,12 @@
       <c r="K41" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L41" s="13"/>
-      <c r="M41" s="13"/>
+      <c r="L41" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="13" t="s">
@@ -2304,8 +2380,12 @@
       <c r="K42" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
+      <c r="L42" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="M42" s="13" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="13" t="s">
@@ -2332,8 +2412,12 @@
       <c r="K43" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="L43" s="13"/>
-      <c r="M43" s="13"/>
+      <c r="L43" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
@@ -2761,10 +2845,10 @@
       <c r="H58" s="16"/>
       <c r="I58" s="16"/>
       <c r="J58" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L58" s="16" t="s">
         <v>98</v>
@@ -4458,464 +4542,524 @@
       <c r="M118" s="19"/>
     </row>
     <row r="119" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B119" s="32" t="s">
+      <c r="B119" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C119" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D119" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E119" s="32"/>
-      <c r="F119" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G119" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H119" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I119" s="32"/>
-      <c r="J119" s="32" t="s">
+      <c r="C119" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D119" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E119" s="16"/>
+      <c r="F119" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G119" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H119" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I119" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J119" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="K119" s="32" t="s">
+      <c r="K119" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="L119" s="16"/>
+      <c r="L119" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="M119" s="16"/>
     </row>
     <row r="120" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B120" s="32" t="s">
+      <c r="B120" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C120" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D120" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E120" s="32"/>
-      <c r="F120" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G120" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H120" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I120" s="32"/>
-      <c r="J120" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K120" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L120" s="16"/>
+      <c r="C120" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D120" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G120" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H120" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I120" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J120" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K120" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L120" s="16" t="s">
+        <v>124</v>
+      </c>
       <c r="M120" s="16"/>
     </row>
     <row r="121" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B121" s="32" t="s">
+      <c r="B121" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C121" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D121" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E121" s="32"/>
-      <c r="F121" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G121" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H121" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I121" s="32"/>
-      <c r="J121" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K121" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L121" s="16"/>
+      <c r="C121" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D121" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G121" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H121" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I121" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J121" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K121" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L121" s="16" t="s">
+        <v>125</v>
+      </c>
       <c r="M121" s="16"/>
     </row>
     <row r="122" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B122" s="32" t="s">
+      <c r="B122" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C122" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E122" s="16"/>
+      <c r="F122" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G122" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H122" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I122" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J122" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K122" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L122" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="M122" s="16"/>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B123" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C123" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G123" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H123" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I123" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J123" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K123" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L123" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="M123" s="16"/>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B124" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C124" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G124" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H124" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I124" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J124" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K124" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L124" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="M124" s="16"/>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B125" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C122" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D122" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G122" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H122" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I122" s="32"/>
-      <c r="J122" s="32" t="s">
+      <c r="C125" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D125" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E125" s="16"/>
+      <c r="F125" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G125" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H125" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I125" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J125" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="K122" s="32" t="s">
+      <c r="K125" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="L122" s="16"/>
-      <c r="M122" s="16"/>
-    </row>
-    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B123" s="32" t="s">
+      <c r="L125" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="M125" s="16"/>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B126" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D126" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G126" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H126" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I126" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J126" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K126" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L126" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="M126" s="16"/>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B127" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C127" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D127" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H127" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I127" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J127" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K127" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L127" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="M127" s="16"/>
+    </row>
+    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B128" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C123" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D123" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E123" s="32"/>
-      <c r="F123" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G123" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H123" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I123" s="32"/>
-      <c r="J123" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K123" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L123" s="16"/>
-      <c r="M123" s="16"/>
-    </row>
-    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B124" s="32" t="s">
+      <c r="C128" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D128" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G128" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H128" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I128" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J128" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K128" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L128" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="M128" s="16"/>
+    </row>
+    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B129" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C124" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D124" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E124" s="32"/>
-      <c r="F124" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G124" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H124" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I124" s="32"/>
-      <c r="J124" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K124" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L124" s="16"/>
-      <c r="M124" s="16"/>
-    </row>
-    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B125" s="12" t="s">
+      <c r="C129" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E129" s="16"/>
+      <c r="F129" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G129" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H129" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I129" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J129" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K129" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L129" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="M129" s="16"/>
+    </row>
+    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B130" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C130" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E130" s="16"/>
+      <c r="F130" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G130" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H130" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I130" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J130" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="K130" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L130" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="M130" s="16"/>
+    </row>
+    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B131" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C125" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D125" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E125" s="12"/>
-      <c r="F125" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G125" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H125" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I125" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J125" s="12" t="s">
+      <c r="C131" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H131" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I131" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J131" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K125" s="12" t="s">
+      <c r="K131" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="L125" s="12"/>
-      <c r="M125" s="12"/>
-    </row>
-    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B126" s="12" t="s">
+      <c r="L131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="M131" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B132" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C126" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D126" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E126" s="12"/>
-      <c r="F126" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G126" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H126" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I126" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="J126" s="12" t="s">
+      <c r="C132" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G132" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H132" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I132" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J132" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K126" s="12" t="s">
+      <c r="K132" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="L126" s="12"/>
-      <c r="M126" s="12"/>
-    </row>
-    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B127" s="12" t="s">
+      <c r="L132" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="M132" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B133" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C127" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D127" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E127" s="12"/>
-      <c r="F127" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G127" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H127" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I127" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J127" s="12" t="s">
+      <c r="C133" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G133" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H133" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I133" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J133" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="K127" s="12" t="s">
+      <c r="K133" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="L127" s="12"/>
-      <c r="M127" s="12"/>
-    </row>
-    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B128" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C128" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D128" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E128" s="32"/>
-      <c r="F128" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G128" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H128" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I128" s="32"/>
-      <c r="J128" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="K128" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="L128" s="16"/>
-      <c r="M128" s="16"/>
-    </row>
-    <row r="129" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B129" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C129" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D129" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E129" s="32"/>
-      <c r="F129" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G129" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H129" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I129" s="32"/>
-      <c r="J129" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K129" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L129" s="16"/>
-      <c r="M129" s="16"/>
-    </row>
-    <row r="130" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B130" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C130" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D130" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E130" s="32"/>
-      <c r="F130" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G130" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H130" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I130" s="32"/>
-      <c r="J130" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K130" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L130" s="16"/>
-      <c r="M130" s="16"/>
-    </row>
-    <row r="131" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B131" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C131" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D131" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E131" s="32"/>
-      <c r="F131" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G131" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H131" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I131" s="32"/>
-      <c r="J131" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="K131" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="L131" s="16"/>
-      <c r="M131" s="16"/>
-    </row>
-    <row r="132" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B132" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C132" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D132" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E132" s="32"/>
-      <c r="F132" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G132" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="H132" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I132" s="32"/>
-      <c r="J132" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K132" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L132" s="16"/>
-      <c r="M132" s="16"/>
-    </row>
-    <row r="133" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B133" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C133" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D133" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E133" s="32"/>
-      <c r="F133" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="G133" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H133" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I133" s="32"/>
-      <c r="J133" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="K133" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="L133" s="16"/>
-      <c r="M133" s="16"/>
+      <c r="L133" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M133" s="12" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="134" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B134" s="32" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C134" s="32" t="s">
         <v>55</v>
@@ -4945,7 +5089,7 @@
     </row>
     <row r="135" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B135" s="32" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C135" s="32" t="s">
         <v>56</v>
@@ -4975,7 +5119,7 @@
     </row>
     <row r="136" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B136" s="32" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C136" s="32" t="s">
         <v>55</v>
@@ -5005,7 +5149,7 @@
     </row>
     <row r="137" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B137" s="32" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>55</v>
@@ -5035,7 +5179,7 @@
     </row>
     <row r="138" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B138" s="32" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C138" s="32" t="s">
         <v>56</v>
@@ -5064,34 +5208,214 @@
       <c r="M138" s="16"/>
     </row>
     <row r="139" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B139" s="33" t="s">
+      <c r="B139" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C139" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D139" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E139" s="32"/>
+      <c r="F139" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G139" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H139" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I139" s="32"/>
+      <c r="J139" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K139" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L139" s="16"/>
+      <c r="M139" s="16"/>
+    </row>
+    <row r="140" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B140" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C140" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D140" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E140" s="32"/>
+      <c r="F140" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G140" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H140" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I140" s="32"/>
+      <c r="J140" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="K140" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L140" s="16"/>
+      <c r="M140" s="16"/>
+    </row>
+    <row r="141" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B141" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C141" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D141" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E141" s="32"/>
+      <c r="F141" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G141" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H141" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I141" s="32"/>
+      <c r="J141" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K141" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L141" s="16"/>
+      <c r="M141" s="16"/>
+    </row>
+    <row r="142" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B142" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C142" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D142" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E142" s="32"/>
+      <c r="F142" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G142" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="H142" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I142" s="32"/>
+      <c r="J142" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K142" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L142" s="16"/>
+      <c r="M142" s="16"/>
+    </row>
+    <row r="143" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B143" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="C139" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D139" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E139" s="33"/>
-      <c r="F139" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="G139" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="H139" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="I139" s="33"/>
-      <c r="J139" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="K139" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="L139" s="24"/>
-      <c r="M139" s="24"/>
+      <c r="C143" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D143" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E143" s="32"/>
+      <c r="F143" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G143" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H143" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I143" s="32"/>
+      <c r="J143" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="K143" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="L143" s="16"/>
+      <c r="M143" s="16"/>
+    </row>
+    <row r="144" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B144" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C144" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D144" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E144" s="32"/>
+      <c r="F144" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="G144" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H144" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I144" s="32"/>
+      <c r="J144" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="K144" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="L144" s="16"/>
+      <c r="M144" s="16"/>
+    </row>
+    <row r="145" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B145" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C145" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D145" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E145" s="33"/>
+      <c r="F145" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G145" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="H145" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="I145" s="33"/>
+      <c r="J145" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K145" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="L145" s="24"/>
+      <c r="M145" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>